<commit_message>
adding rev 0.1 of sensor board pcb
</commit_message>
<xml_diff>
--- a/Water-Probe/Design Files/Production Files/BoSL-Probe BOM.xlsx
+++ b/Water-Probe/Design Files/Production Files/BoSL-Probe BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data\My Documents\Monash\Monash-BoSL\Water-Probe\Design Files\Production Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23AC223D-EF9C-4EF1-8F8A-B429F43646B9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2B6703B-5E7E-4DBC-A624-20FC341A5E11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>Part Number</t>
   </si>
@@ -87,15 +87,9 @@
     <t>Total Price</t>
   </si>
   <si>
-    <t>(preferably with metal)</t>
-  </si>
-  <si>
     <t>Threaded Rod</t>
   </si>
   <si>
-    <t>4-40 Tread | 35mm length</t>
-  </si>
-  <si>
     <t>Resistor</t>
   </si>
   <si>
@@ -109,6 +103,24 @@
   </si>
   <si>
     <t>6 m</t>
+  </si>
+  <si>
+    <t>4-40 Thread | 35mm length</t>
+  </si>
+  <si>
+    <t>to-92 heatsink</t>
+  </si>
+  <si>
+    <t>https://au.element14.com/aavid-thermalloy/575200b00000g/heat-sink-aluminium/dp/2822615?st=to-92%20heatsink</t>
+  </si>
+  <si>
+    <t>Heatsink</t>
+  </si>
+  <si>
+    <t>to-92</t>
+  </si>
+  <si>
+    <t>https://au.element14.com/maxim-integrated-products/ds18b20/temperature-sensor/dp/2515553?st=ds18b20</t>
   </si>
 </sst>
 </file>
@@ -215,17 +227,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -506,15 +518,16 @@
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="36.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" style="10" customWidth="1"/>
     <col min="3" max="3" width="29.7109375" customWidth="1"/>
     <col min="4" max="4" width="28.42578125" customWidth="1"/>
+    <col min="6" max="7" width="8.85546875" style="11"/>
     <col min="8" max="8" width="57.5703125" customWidth="1"/>
     <col min="9" max="9" width="18.42578125" customWidth="1"/>
   </cols>
@@ -523,7 +536,7 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -535,10 +548,10 @@
       <c r="E1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="16" t="s">
         <v>18</v>
       </c>
       <c r="H1" t="s">
@@ -546,10 +559,9 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="15">
+      <c r="A2" s="10">
         <v>7774</v>
       </c>
-      <c r="B2" s="6"/>
       <c r="C2" t="s">
         <v>14</v>
       </c>
@@ -559,12 +571,14 @@
       <c r="E2">
         <v>2</v>
       </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16">
+      <c r="F2" s="11">
+        <v>0.66</v>
+      </c>
+      <c r="G2" s="11">
         <f>E2*F2</f>
-        <v>0</v>
-      </c>
-      <c r="H2" s="13" t="s">
+        <v>1.32</v>
+      </c>
+      <c r="H2" s="9" t="s">
         <v>12</v>
       </c>
     </row>
@@ -572,65 +586,69 @@
       <c r="A3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="6"/>
       <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
       <c r="E3">
         <v>1</v>
       </c>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16">
+      <c r="F3" s="11">
+        <v>4.49</v>
+      </c>
+      <c r="G3" s="11">
         <f t="shared" ref="G3:G4" si="0">E3*F3</f>
-        <v>0</v>
-      </c>
-      <c r="H3" s="13"/>
+        <v>4.49</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="7"/>
+      <c r="B4" s="12"/>
       <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="11">
         <v>19</v>
       </c>
-      <c r="G4" s="16">
+      <c r="G4" s="11">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1"/>
-      <c r="B5" s="7"/>
+      <c r="B5" s="12"/>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E5">
         <v>2</v>
       </c>
+      <c r="G5" s="11">
+        <f>F5*E5</f>
+        <v>0</v>
+      </c>
       <c r="H5" s="4"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="15" t="s">
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
@@ -638,31 +656,39 @@
       <c r="E6">
         <v>2</v>
       </c>
+      <c r="G6" s="11">
+        <f t="shared" ref="G6:G10" si="1">F6*E6</f>
+        <v>0</v>
+      </c>
       <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1"/>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="15" t="s">
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
+      <c r="G7" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1"/>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="12" t="s">
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
         <v>8</v>
@@ -670,125 +696,153 @@
       <c r="E8">
         <v>1</v>
       </c>
+      <c r="G8" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="B9" s="7"/>
+      <c r="B9" s="12"/>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
+      <c r="G9" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="B10" s="7"/>
-      <c r="H10" s="4"/>
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" s="11">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G10" s="11">
+        <f t="shared" si="1"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="B11" s="7"/>
+      <c r="B11" s="12"/>
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="B12" s="7"/>
+      <c r="B12" s="12"/>
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="B13" s="7"/>
+      <c r="B13" s="12"/>
       <c r="H13" s="3"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="2"/>
-      <c r="B14" s="7"/>
+      <c r="B14" s="12"/>
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="B15" s="7"/>
+      <c r="B15" s="12"/>
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="B16" s="7"/>
+      <c r="B16" s="12"/>
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="B17" s="7"/>
+      <c r="B17" s="12"/>
       <c r="H17" s="4"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="B18" s="7"/>
+      <c r="B18" s="12"/>
       <c r="H18" s="3"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="B19" s="7"/>
+      <c r="B19" s="12"/>
       <c r="H19" s="3"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="B20" s="7"/>
+      <c r="B20" s="12"/>
       <c r="H20" s="3"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="B21" s="7"/>
+      <c r="B21" s="12"/>
       <c r="H21" s="3"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="B22" s="7"/>
+      <c r="B22" s="12"/>
       <c r="H22" s="3"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="B23" s="7"/>
+      <c r="B23" s="12"/>
       <c r="H23" s="4"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="B24" s="7"/>
+      <c r="B24" s="12"/>
       <c r="H24" s="4"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="B25" s="7"/>
+      <c r="B25" s="12"/>
       <c r="H25" s="4"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="B26" s="7"/>
-      <c r="H26" s="9"/>
+      <c r="B26" s="12"/>
+      <c r="H26" s="6"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="B27" s="7"/>
-      <c r="H27" s="13"/>
+      <c r="B27" s="12"/>
+      <c r="H27" s="9"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="10"/>
-      <c r="B28" s="11"/>
-      <c r="H28" s="9"/>
+      <c r="A28" s="7"/>
+      <c r="B28" s="13"/>
+      <c r="H28" s="6"/>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="1"/>
-      <c r="B29" s="11"/>
-      <c r="H29" s="13"/>
+      <c r="B29" s="13"/>
+      <c r="H29" s="9"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="12"/>
-      <c r="B30" s="11"/>
-      <c r="H30" s="9"/>
+      <c r="A30" s="8"/>
+      <c r="B30" s="13"/>
+      <c r="H30" s="6"/>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="1"/>
       <c r="B31" s="14"/>
-      <c r="H31" s="9"/>
+      <c r="H31" s="6"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="B32" s="3"/>
+      <c r="B32" s="12"/>
       <c r="H32" s="3"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="10"/>
-      <c r="C33" s="10"/>
+      <c r="A33" s="7"/>
+      <c r="C33" s="7"/>
       <c r="H33" s="3"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="B34" s="3"/>
+      <c r="B34" s="12"/>
       <c r="H34" s="3"/>
     </row>
     <row r="35" spans="1:8">
@@ -803,8 +857,9 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H4" r:id="rId1" xr:uid="{F051EB1A-1700-4F0F-B96E-5AEEE4454916}"/>
+    <hyperlink ref="H2" r:id="rId2" xr:uid="{C1B8C97B-04F6-4323-9D0A-161D051640C8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
transmit code added to gps
</commit_message>
<xml_diff>
--- a/Water-Probe/Design Files/Production Files/BoSL-Probe BOM.xlsx
+++ b/Water-Probe/Design Files/Production Files/BoSL-Probe BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data\My Documents\Monash\Monash-BoSL\Water-Probe\Design Files\Production Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40CEE6A6-5CED-4477-BD20-7D9BB0286436}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E600E29C-D2A3-4FB0-AFFC-7252506F6BEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,12 +66,6 @@
     <t>0805</t>
   </si>
   <si>
-    <t>https://www.digikey.com.au/product-detail/en/keystone-electronics/7774/36-7774-ND/2745944</t>
-  </si>
-  <si>
-    <t>4-40 Thread</t>
-  </si>
-  <si>
     <t>Screw Terminal</t>
   </si>
   <si>
@@ -87,9 +81,6 @@
     <t>Total Price</t>
   </si>
   <si>
-    <t>Threaded Rod</t>
-  </si>
-  <si>
     <t>Resistor</t>
   </si>
   <si>
@@ -99,22 +90,31 @@
     <t>Capactor</t>
   </si>
   <si>
-    <t>4-40 Thread | 35mm length</t>
-  </si>
-  <si>
-    <t>to-92 heatsink</t>
-  </si>
-  <si>
-    <t>https://au.element14.com/aavid-thermalloy/575200b00000g/heat-sink-aluminium/dp/2822615?st=to-92%20heatsink</t>
-  </si>
-  <si>
-    <t>Heatsink</t>
-  </si>
-  <si>
-    <t>to-92</t>
-  </si>
-  <si>
     <t>https://au.element14.com/maxim-integrated-products/ds18b20/temperature-sensor/dp/2515553?st=ds18b20</t>
+  </si>
+  <si>
+    <t>3 Screw Terminal</t>
+  </si>
+  <si>
+    <t>Metal Cap</t>
+  </si>
+  <si>
+    <t>Stainless Steel Dowel Pin</t>
+  </si>
+  <si>
+    <t>3.5mm pitch</t>
+  </si>
+  <si>
+    <t>https://au.element14.com/camdenboss/ctbp3051-3/tb-wire-to-board-3pos-24-18awg/dp/2527546?st=3%20terminal%20block</t>
+  </si>
+  <si>
+    <t>Eithernet Cable</t>
+  </si>
+  <si>
+    <t>2.5 m</t>
+  </si>
+  <si>
+    <t>35 mm Length 1/16" dia</t>
   </si>
 </sst>
 </file>
@@ -500,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -534,45 +534,46 @@
         <v>10</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="9">
-        <v>7774</v>
+      <c r="A2" s="9"/>
+      <c r="B2" s="9" t="s">
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2" s="10">
-        <v>0.66</v>
+        <v>2.2400000000000002</v>
       </c>
       <c r="G2" s="10">
         <f>E2*F2</f>
-        <v>1.32</v>
+        <v>2.2400000000000002</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -585,7 +586,7 @@
         <v>4.49</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -611,52 +612,54 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="1"/>
-      <c r="B5" s="11"/>
+      <c r="B5" s="14" t="s">
+        <v>11</v>
+      </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="E5">
         <v>2</v>
       </c>
       <c r="G5" s="10">
-        <f>F5*E5</f>
+        <f t="shared" ref="G5:G7" si="1">F5*E5</f>
         <v>0</v>
       </c>
       <c r="H5" s="4"/>
     </row>
     <row r="6" spans="1:8">
+      <c r="A6" s="1"/>
       <c r="B6" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6" s="10">
-        <f t="shared" ref="G6:G9" si="1">F6*E6</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1"/>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -668,69 +671,65 @@
       <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="1"/>
-      <c r="B8" s="11" t="s">
-        <v>11</v>
-      </c>
+      <c r="B8" s="11"/>
       <c r="C8" t="s">
         <v>22</v>
       </c>
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
       <c r="E8">
         <v>1</v>
       </c>
-      <c r="G8" s="10">
-        <f t="shared" si="1"/>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="B9" s="11"/>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="G9" s="10">
+        <f>F9*E9</f>
         <v>0</v>
       </c>
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9" s="10">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G9" s="10">
-        <f t="shared" si="1"/>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:8">
       <c r="B10" s="11"/>
-      <c r="H10" s="4"/>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="G10" s="10">
+        <f>F10*E10</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:8">
       <c r="B11" s="11"/>
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8">
+      <c r="A12" s="2"/>
       <c r="B12" s="11"/>
-      <c r="H12" s="3"/>
+      <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="2"/>
       <c r="B13" s="11"/>
-      <c r="H13" s="4"/>
+      <c r="H13" s="3"/>
     </row>
     <row r="14" spans="1:8">
       <c r="B14" s="11"/>
-      <c r="H14" s="3"/>
+      <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8">
       <c r="B15" s="11"/>
@@ -738,7 +737,7 @@
     </row>
     <row r="16" spans="1:8">
       <c r="B16" s="11"/>
-      <c r="H16" s="4"/>
+      <c r="H16" s="3"/>
     </row>
     <row r="17" spans="1:8">
       <c r="B17" s="11"/>
@@ -758,7 +757,7 @@
     </row>
     <row r="21" spans="1:8">
       <c r="B21" s="11"/>
-      <c r="H21" s="3"/>
+      <c r="H21" s="4"/>
     </row>
     <row r="22" spans="1:8">
       <c r="B22" s="11"/>
@@ -770,62 +769,58 @@
     </row>
     <row r="24" spans="1:8">
       <c r="B24" s="11"/>
-      <c r="H24" s="4"/>
+      <c r="H24" s="5"/>
     </row>
     <row r="25" spans="1:8">
       <c r="B25" s="11"/>
-      <c r="H25" s="5"/>
+      <c r="H25" s="8"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="B26" s="11"/>
-      <c r="H26" s="8"/>
+      <c r="A26" s="6"/>
+      <c r="B26" s="12"/>
+      <c r="H26" s="5"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="6"/>
+      <c r="A27" s="1"/>
       <c r="B27" s="12"/>
-      <c r="H27" s="5"/>
+      <c r="H27" s="8"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="1"/>
+      <c r="A28" s="7"/>
       <c r="B28" s="12"/>
-      <c r="H28" s="8"/>
+      <c r="H28" s="5"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="7"/>
-      <c r="B29" s="12"/>
+      <c r="A29" s="1"/>
+      <c r="B29" s="13"/>
       <c r="H29" s="5"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="1"/>
-      <c r="B30" s="13"/>
-      <c r="H30" s="5"/>
+      <c r="B30" s="11"/>
+      <c r="H30" s="3"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="B31" s="11"/>
+      <c r="A31" s="6"/>
+      <c r="C31" s="6"/>
       <c r="H31" s="3"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="6"/>
-      <c r="C32" s="6"/>
+      <c r="B32" s="11"/>
       <c r="H32" s="3"/>
     </row>
-    <row r="33" spans="2:8">
-      <c r="B33" s="11"/>
+    <row r="33" spans="8:8">
       <c r="H33" s="3"/>
     </row>
-    <row r="34" spans="2:8">
+    <row r="34" spans="8:8">
       <c r="H34" s="3"/>
     </row>
-    <row r="35" spans="2:8">
+    <row r="35" spans="8:8">
       <c r="H35" s="3"/>
-    </row>
-    <row r="36" spans="2:8">
-      <c r="H36" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H4" r:id="rId1" xr:uid="{F051EB1A-1700-4F0F-B96E-5AEEE4454916}"/>
-    <hyperlink ref="H2" r:id="rId2" xr:uid="{C1B8C97B-04F6-4323-9D0A-161D051640C8}"/>
+    <hyperlink ref="H2" r:id="rId2" xr:uid="{36E8689D-39A3-4B7C-8137-46FD67F92DCD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>

</xml_diff>

<commit_message>
ammened partlist for all-in-one probe
</commit_message>
<xml_diff>
--- a/Water-Probe/Design Files/Production Files/BoSL-Probe BOM.xlsx
+++ b/Water-Probe/Design Files/Production Files/BoSL-Probe BOM.xlsx
@@ -1,34 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20343"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data\My Documents\Monash\Monash-BoSL\Water-Probe\Design Files\Production Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ad.monash.edu\home\User070\scat0009\Documents\Monash-BoSL\Water-Probe\Design Files\Production Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E600E29C-D2A3-4FB0-AFFC-7252506F6BEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F39735F-C2D7-49C6-AB07-B532FC802FA6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>Part Number</t>
   </si>
@@ -115,6 +107,9 @@
   </si>
   <si>
     <t>35 mm Length 1/16" dia</t>
+  </si>
+  <si>
+    <t>Silicon Eithernet Wires to PCB</t>
   </si>
 </sst>
 </file>
@@ -500,21 +495,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="36.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="29.7109375" customWidth="1"/>
-    <col min="4" max="4" width="28.42578125" customWidth="1"/>
-    <col min="6" max="7" width="8.85546875" style="10"/>
-    <col min="8" max="8" width="57.5703125" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="36.5546875" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="29.6640625" customWidth="1"/>
+    <col min="4" max="4" width="28.44140625" customWidth="1"/>
+    <col min="6" max="7" width="8.88671875" style="10"/>
+    <col min="8" max="8" width="57.5546875" customWidth="1"/>
+    <col min="9" max="9" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -683,53 +678,56 @@
     <row r="9" spans="1:8">
       <c r="B9" s="11"/>
       <c r="C9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
-      <c r="G9" s="10">
-        <f>F9*E9</f>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:8">
       <c r="B10" s="11"/>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G10" s="10">
         <f>F10*E10</f>
         <v>0</v>
       </c>
-      <c r="H10" s="3"/>
+      <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8">
       <c r="B11" s="11"/>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="G11" s="10">
+        <f>F11*E11</f>
+        <v>0</v>
+      </c>
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="2"/>
       <c r="B12" s="11"/>
-      <c r="H12" s="4"/>
+      <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8">
+      <c r="A13" s="2"/>
       <c r="B13" s="11"/>
-      <c r="H13" s="3"/>
+      <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:8">
       <c r="B14" s="11"/>
-      <c r="H14" s="4"/>
+      <c r="H14" s="3"/>
     </row>
     <row r="15" spans="1:8">
       <c r="B15" s="11"/>
@@ -737,7 +735,7 @@
     </row>
     <row r="16" spans="1:8">
       <c r="B16" s="11"/>
-      <c r="H16" s="3"/>
+      <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:8">
       <c r="B17" s="11"/>
@@ -757,7 +755,7 @@
     </row>
     <row r="21" spans="1:8">
       <c r="B21" s="11"/>
-      <c r="H21" s="4"/>
+      <c r="H21" s="3"/>
     </row>
     <row r="22" spans="1:8">
       <c r="B22" s="11"/>
@@ -769,53 +767,57 @@
     </row>
     <row r="24" spans="1:8">
       <c r="B24" s="11"/>
-      <c r="H24" s="5"/>
+      <c r="H24" s="4"/>
     </row>
     <row r="25" spans="1:8">
       <c r="B25" s="11"/>
-      <c r="H25" s="8"/>
+      <c r="H25" s="5"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="6"/>
-      <c r="B26" s="12"/>
-      <c r="H26" s="5"/>
+      <c r="B26" s="11"/>
+      <c r="H26" s="8"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="1"/>
+      <c r="A27" s="6"/>
       <c r="B27" s="12"/>
-      <c r="H27" s="8"/>
+      <c r="H27" s="5"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="7"/>
+      <c r="A28" s="1"/>
       <c r="B28" s="12"/>
-      <c r="H28" s="5"/>
+      <c r="H28" s="8"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="1"/>
-      <c r="B29" s="13"/>
+      <c r="A29" s="7"/>
+      <c r="B29" s="12"/>
       <c r="H29" s="5"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="B30" s="11"/>
-      <c r="H30" s="3"/>
+      <c r="A30" s="1"/>
+      <c r="B30" s="13"/>
+      <c r="H30" s="5"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="6"/>
-      <c r="C31" s="6"/>
+      <c r="B31" s="11"/>
       <c r="H31" s="3"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="B32" s="11"/>
+      <c r="A32" s="6"/>
+      <c r="C32" s="6"/>
       <c r="H32" s="3"/>
     </row>
-    <row r="33" spans="8:8">
+    <row r="33" spans="2:8">
+      <c r="B33" s="11"/>
       <c r="H33" s="3"/>
     </row>
-    <row r="34" spans="8:8">
+    <row r="34" spans="2:8">
       <c r="H34" s="3"/>
     </row>
-    <row r="35" spans="8:8">
+    <row r="35" spans="2:8">
       <c r="H35" s="3"/>
+    </row>
+    <row r="36" spans="2:8">
+      <c r="H36" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>